<commit_message>
updated spreadsheet - minor additional saves
</commit_message>
<xml_diff>
--- a/data/flat_text/labeling_ground_truth.xlsx
+++ b/data/flat_text/labeling_ground_truth.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\LLM-Safety-Mechanisms\data\flat_text\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F1D826A-6539-458A-9E9B-99BDAC8250F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F923456B-81EE-40DA-AB0F-32301ED811EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="25490" yWindow="-110" windowWidth="19420" windowHeight="11020" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2687" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2702" uniqueCount="177">
   <si>
     <t>LLM Safety Mechanisms - Ground Truth Labeling Template</t>
   </si>
@@ -554,6 +554,9 @@
   </si>
   <si>
     <t>explicit part of overall strategy</t>
+  </si>
+  <si>
+    <t>References a plot showing win rates for adversarial scenarios</t>
   </si>
 </sst>
 </file>
@@ -1115,10 +1118,10 @@
   <dimension ref="A1:H488"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B18" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B460" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F40" sqref="F40"/>
+      <selection pane="bottomRight" activeCell="A485" sqref="A485"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2246,8 +2249,12 @@
       <c r="E46" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="F46" s="3"/>
-      <c r="G46" s="3"/>
+      <c r="F46" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="G46" s="3" t="s">
+        <v>163</v>
+      </c>
       <c r="H46" s="3"/>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.35">
@@ -2266,9 +2273,15 @@
       <c r="E47" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="F47" s="3"/>
-      <c r="G47" s="3"/>
-      <c r="H47" s="3"/>
+      <c r="F47" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="G47" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="H47" s="3" t="s">
+        <v>176</v>
+      </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A48" s="3" t="s">
@@ -2286,8 +2299,12 @@
       <c r="E48" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="F48" s="3"/>
-      <c r="G48" s="3"/>
+      <c r="F48" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="G48" s="3" t="s">
+        <v>163</v>
+      </c>
       <c r="H48" s="3"/>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.35">
@@ -2306,8 +2323,12 @@
       <c r="E49" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="F49" s="3"/>
-      <c r="G49" s="3"/>
+      <c r="F49" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="G49" s="3" t="s">
+        <v>163</v>
+      </c>
       <c r="H49" s="3"/>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.35">
@@ -2326,8 +2347,12 @@
       <c r="E50" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="F50" s="3"/>
-      <c r="G50" s="3"/>
+      <c r="F50" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="G50" s="3" t="s">
+        <v>163</v>
+      </c>
       <c r="H50" s="3"/>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.35">
@@ -2346,8 +2371,12 @@
       <c r="E51" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="F51" s="3"/>
-      <c r="G51" s="3"/>
+      <c r="F51" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="G51" s="3" t="s">
+        <v>163</v>
+      </c>
       <c r="H51" s="3"/>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.35">
@@ -2366,8 +2395,12 @@
       <c r="E52" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="F52" s="3"/>
-      <c r="G52" s="3"/>
+      <c r="F52" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="G52" s="3" t="s">
+        <v>163</v>
+      </c>
       <c r="H52" s="3"/>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.35">

</xml_diff>